<commit_message>
Aggiornato file excel con status elaborazioni
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -37,31 +37,37 @@
     <t xml:space="preserve">Abruzzo</t>
   </si>
   <si>
+    <t xml:space="preserve">Non completato. Chiesto al Centro Funzionale un’anagrafica delle stazioni</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati ricevuti da Cesolari (Centro Funzionale Abruzzo)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aeronautica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completato controlli qualità interni e controlli spaziali</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati acquisiti da Guido tramite ftp da NOAA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolzano</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non completato</t>
   </si>
   <si>
-    <t xml:space="preserve">Dati ricevuti da Cesolari (Centro Funzionale Abruzzo)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Aeronautica</t>
+    <t xml:space="preserve">Le serie si interrompono a novembre 2017, ricontrollare più avanti se ci sono aggiornamenti delle serie. Attenzione: la serie 56900MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 56800MS. La serie 39100MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 69600MS. La serie 37100MS sembra non corrispondere ad alcuna serie.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lazio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marche</t>
   </si>
   <si>
     <t xml:space="preserve">Completato controlli qualità interni</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dati acquisiti da Guido tramite ftp da NOAA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bolzano</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le serie si interrompono a novembre 2017, ricontrollare più avanti se ci sono aggiornamenti delle serie. Attenzione: la serie 56900MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 56800MS. La serie 39100MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 69600MS. La serie 37100MS sembra non corrispondere ad alcuna serie.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lazio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marche</t>
   </si>
   <si>
     <t xml:space="preserve">Dati ricevuti da Centro Funzionale Marche</t>
@@ -89,6 +95,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,6 +117,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -178,11 +186,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -265,13 +273,13 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.62"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
@@ -290,17 +298,17 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="n">
-        <v>43139</v>
+        <v>43140</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="5" t="s">
         <v>6</v>
       </c>
     </row>
@@ -309,12 +317,12 @@
         <v>7</v>
       </c>
       <c r="B3" s="3" t="n">
-        <v>43139</v>
+        <v>43140</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -325,63 +333,63 @@
       <c r="B4" s="3" t="n">
         <v>43139</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="5" t="s">
+      <c r="C4" s="5" t="s">
         <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>43139</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>43139</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>14</v>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>43139</v>
       </c>
-      <c r="C7" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="4"/>
+      <c r="C7" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>43139</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>17</v>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finiti controlli spaziali di Toscana e Marche
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t xml:space="preserve">Marche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Completato controlli qualità interni</t>
   </si>
   <si>
     <t xml:space="preserve">Dati ricevuti da Centro Funzionale Marche</t>
@@ -273,7 +270,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -357,30 +354,30 @@
         <v>14</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>43139</v>
+        <v>43143</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>43139</v>
+        <v>43143</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="D7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>43139</v>
@@ -389,7 +386,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento situazione elaborazione e aggiunta colonna con siti web delle fonti
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">Nota</t>
   </si>
   <si>
+    <t xml:space="preserve">Fonte Dati</t>
+  </si>
+  <si>
     <t xml:space="preserve">Abruzzo</t>
   </si>
   <si>
@@ -52,24 +55,48 @@
     <t xml:space="preserve">Dati acquisiti da Guido tramite ftp da NOAA</t>
   </si>
   <si>
+    <t xml:space="preserve">ftp.ncdc.noaa.gov/pub/data/gsod</t>
+  </si>
+  <si>
     <t xml:space="preserve">Basilicata</t>
   </si>
   <si>
+    <t xml:space="preserve">Sono state acquisite dal sito web solo tre serie di temperatura che facilmente sono state associate alle serie disponibili</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.centrofunzionalebasilicata.it/it/scaricaDati.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bolzano</t>
+  </si>
+  <si>
     <t xml:space="preserve">Non completato</t>
   </si>
   <si>
-    <t xml:space="preserve">Bolzano</t>
-  </si>
-  <si>
     <t xml:space="preserve">Le serie si interrompono a novembre 2017, ricontrollare più avanti se ci sono aggiornamenti delle serie. Attenzione: la serie 56900MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 56800MS. La serie 39100MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 69600MS. La serie 37100MS sembra non corrispondere ad alcuna serie.</t>
   </si>
   <si>
     <t xml:space="preserve">Calabria</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.cfd.calabria.it/index.php/dati-stazioni/dati-storici</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Campania</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Al momento le serie disponibili on-line sono quelle fino a dicembre 2016. Il programma per lo scarico dei dati si blocca di continuo (o meglio il server sembra staccare il programma). Per questo motivo il programma è stato scritto in modo di salvare su file ogni anno acquisito di ciascuna stazione, processo abbastanza lento. Le serie sul sito del Centro Funzionale hanno un codice identificativo che NON corrisponde a quello di HisCentral. Per associare le serie del Centro Funzionale a quelle di His Central sono state scaricate le serie per l’anno 2014 (solo per un anno, perché dal 2000 il programma ci avrebbe messo troppo, scarica molto lentamente, si blocca di continuo). Quindi le serie per il 2014 sono state confrontate con quelle di HisCentral e le associazioni tra codici riportate nel file di anagrafica. Una volta ottenuta la corretta associazione tra codici (e nomi stazion) sono stati scaricati i dati per il 2015 e il 2016.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://centrofunzionale.regione.campania.it/#/pages/sensori</t>
+  </si>
+  <si>
     <t xml:space="preserve">Lazio</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.idrografico.roma.it/annali/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marche</t>
   </si>
   <si>
@@ -79,10 +106,16 @@
     <t xml:space="preserve">Toscana</t>
   </si>
   <si>
+    <t xml:space="preserve">http://www.sir.toscana.it/</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valle d’Aosta</t>
   </si>
   <si>
     <t xml:space="preserve">Dati acquisiti da sito web Centro Funzionale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://cf.regione.vda.it/il_centro_funzionale.php</t>
   </si>
 </sst>
 </file>
@@ -91,7 +124,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="MM/DD/YY"/>
+    <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -171,7 +204,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -193,6 +226,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -273,10 +310,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,7 +321,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.2"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -300,123 +338,166 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>43140</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>6</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>43140</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>43153</v>
+        <v>43172</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>43139</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>43152</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="225.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="B7" s="3" t="n">
-        <v>43139</v>
+        <v>43172</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>43143</v>
+        <v>43139</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>17</v>
+        <v>9</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>43143</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B10" s="3" t="n">
+        <v>43143</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="5"/>
+      <c r="E10" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="3" t="n">
         <v>43145</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>20</v>
+      <c r="C11" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento informazioni su Umbria e Bolzano
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -70,9 +70,6 @@
     <t xml:space="preserve">Bolzano</t>
   </si>
   <si>
-    <t xml:space="preserve">Non completato</t>
-  </si>
-  <si>
     <t xml:space="preserve">Le serie si interrompono a novembre 2017, ricontrollare più avanti se ci sono aggiornamenti delle serie. Attenzione: la serie 56900MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 56800MS. La serie 39100MS non compare in anagrafica ma dovrebbe corrispondere alla serie di HisCentral 69600MS. La serie 37100MS sembra non corrispondere ad alcuna serie.</t>
   </si>
   <si>
@@ -116,15 +113,28 @@
   </si>
   <si>
     <t xml:space="preserve">http://cf.regione.vda.it/il_centro_funzionale.php</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umbria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non completato. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati 2016 e 2017 acquisiti da Centro Funzionale Umbria; Dati precipitazione 2014 ricevuti via fax da Centro Funzionale Umbria, Dati temperatura 2014: richiesti via fax ma sono state inviate solo le temperature medie, quindi al momento mancano le massime e le minime per il 2014. Sul sito del Centro Funzionale (nei pdf) i nomi non sempre corrispondono ai nomi delle stazioni in anagrafica. Per le stazioni senza corrispondenza esatta è stata fatta una ricerca su google maps e sulle mappe con le ubicazioni delle stazioni sul sito del Centro Funzionale.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">http://www.regione.umbria.it/ambiente/servizio-idrografico</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -204,7 +214,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -231,6 +241,14 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -310,10 +328,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -396,19 +414,19 @@
         <v>15</v>
       </c>
       <c r="B5" s="3" t="n">
-        <v>43139</v>
+        <v>43173</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>17</v>
       </c>
       <c r="E5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>43152</v>
@@ -418,12 +436,12 @@
       </c>
       <c r="D6" s="4"/>
       <c r="E6" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="225.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>43172</v>
@@ -432,15 +450,15 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="6" t="s">
         <v>21</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>43139</v>
@@ -450,12 +468,12 @@
       </c>
       <c r="D8" s="5"/>
       <c r="E8" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>43143</v>
@@ -464,13 +482,13 @@
         <v>9</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="n">
         <v>43143</v>
@@ -480,12 +498,12 @@
       </c>
       <c r="D10" s="5"/>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="3" t="n">
         <v>43145</v>
@@ -494,10 +512,27 @@
         <v>9</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E11" s="6" t="s">
+    </row>
+    <row r="12" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
         <v>31</v>
+      </c>
+      <c r="B12" s="7" t="n">
+        <v>43173</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornato file excel con Umbria
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="34">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -116,9 +116,6 @@
   </si>
   <si>
     <t xml:space="preserve">Umbria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non completato. </t>
   </si>
   <si>
     <t xml:space="preserve">Dati 2016 e 2017 acquisiti da Centro Funzionale Umbria; Dati precipitazione 2014 ricevuti via fax da Centro Funzionale Umbria, Dati temperatura 2014: richiesti via fax ma sono state inviate solo le temperature medie, quindi al momento mancano le massime e le minime per il 2014. Sul sito del Centro Funzionale (nei pdf) i nomi non sempre corrispondono ai nomi delle stazioni in anagrafica. Per le stazioni senza corrispondenza esatta è stata fatta una ricerca su google maps e sulle mappe con le ubicazioni delle stazioni sul sito del Centro Funzionale.</t>
@@ -131,10 +128,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="DD/MM/YY"/>
-    <numFmt numFmtId="166" formatCode="DD/MM/YY"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -214,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -240,10 +236,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,8 +322,8 @@
   </sheetPr>
   <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -522,17 +514,17 @@
       <c r="A12" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="7" t="n">
-        <v>43173</v>
-      </c>
-      <c r="C12" s="0" t="s">
+      <c r="B12" s="3" t="n">
+        <v>43174</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="E12" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
aggiornamento status elaborazione serie, Emilia Romagna
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -83,6 +83,12 @@
   </si>
   <si>
     <t xml:space="preserve">http://centrofunzionale.regione.campania.it/#/pages/sensori</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Emilia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dati del 2016 acquisiti da HisCentral, Dati del 2017 ricavati da serie limitrofe a quelle di HisCentral. Sono state estese al 2017 solo le serie che appartengono al gruppo di serie tmax/tmin omogenizzate mediante Climatol. Per questo gruppo di sottostazioni omogenee dell’Emilia (circa 19) sono state individuate (in un raggio di 25km e con una differenza di quota di circa 100 metri) sette stazioni limitrofe.COD_STAZ==1,9013; COD_STAZ==7097,9200;COD_STAZ==7098,9277;COD_STAZ==7102,9146;COD_STAZ==7112,9225;COD_STAZ==7118,9314;COD_STAZ==7127,9588;COD_STAZ==8,9139. I codici superiori a 9000 identificano le serie di HisCentral.</t>
   </si>
   <si>
     <t xml:space="preserve">Lazio</t>
@@ -317,10 +323,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -445,35 +451,35 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="225.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B8" s="3" t="n">
-        <v>43139</v>
+        <v>43235</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6" t="s">
+      <c r="D8" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B9" s="3" t="n">
-        <v>43143</v>
+        <v>43139</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -485,43 +491,58 @@
       <c r="C10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>26</v>
       </c>
+      <c r="E10" s="6"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
         <v>27</v>
       </c>
       <c r="B11" s="3" t="n">
+        <v>43143</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="5"/>
+      <c r="E11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B12" s="3" t="n">
         <v>43145</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
+      <c r="C12" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="3" t="n">
+      <c r="E12" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="120" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="3" t="n">
         <v>43174</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>32</v>
+      <c r="C13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Aggiornamento del file excel sulla situazione delle serie giornaliere
</commit_message>
<xml_diff>
--- a/status_serie_giornaliere.xlsx
+++ b/status_serie_giornaliere.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t xml:space="preserve">Centro Funzionale</t>
   </si>
@@ -28,9 +28,6 @@
     <t xml:space="preserve">Ultima rilevazione</t>
   </si>
   <si>
-    <t xml:space="preserve">Elaborazione</t>
-  </si>
-  <si>
     <t xml:space="preserve">Nota</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t xml:space="preserve">Abruzzo</t>
   </si>
   <si>
-    <t xml:space="preserve">Completato controlli qualità interni e controlli spaziali</t>
-  </si>
-  <si>
     <t xml:space="preserve">Dati ricevuti da Cesolari (Centro Funzionale Abruzzo)</t>
   </si>
   <si>
@@ -94,6 +88,12 @@
     <t xml:space="preserve">Lazio</t>
   </si>
   <si>
+    <t xml:space="preserve">17/08/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nel 2019 I dati del Lazio sono stati passati da Walter in quanto il sito dell’Idrografico Regione Lazio era fuori servizio. A fine 2019 il sito era nuovamente funzionante. Dal sito (nel 2020) sono state acquisite le serie del 2018 e sostituite a quelle passate nel 2019 da Walter. I valori forniti da Walter e quelli dell’Idrografico erano pressoche gli stessi ma non esattamente uguali. Per I valori 2019 il sito dell’Idrografico non ha ancora fornito I dati giornalieri. Tuttavia questi sono disponibili presso la sezione OpenData del Lazio che oggi (17 febbraio 2020) ha caricato anche I dati di pioggia per dicembre 2019, completando cos’ la serie del 2019. I dati OpenData 2018 sono stati confrontati con I dati 2018 acquisiti dal sito dell’Idrografico. I valori sono esattamente gli stessi.</t>
+  </si>
+  <si>
     <t xml:space="preserve">http://www.idrografico.roma.it/annali/</t>
   </si>
   <si>
@@ -112,7 +112,7 @@
     <t xml:space="preserve">Valle d’Aosta</t>
   </si>
   <si>
-    <t xml:space="preserve">Dati acquisiti da sito web Centro Funzionale</t>
+    <t xml:space="preserve">Dati acquisiti da sito web Centro Funzionale. Nel 2019/2020 il sito del Centro Funzionale VdA ha cambiato interfaccia e formato dati. I dati sub giornalieri erano disponibili in formato semi-orario (ogni 30 minut). Da fine 2019 I dati sono disponibili solo I dati in formato orario e giornaliero. Questo non permette di ricostruire piu’ esattamente la stessa aggregazione delle serie storiche ma non esiste altra soluzione al problema.</t>
   </si>
   <si>
     <t xml:space="preserve">http://cf.regione.vda.it/il_centro_funzionale.php</t>
@@ -231,10 +231,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -243,17 +239,21 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -323,19 +323,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="23.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="48.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="57.94"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="48.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.94"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -351,133 +350,108 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>43140</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6"/>
+        <v>5</v>
+      </c>
+      <c r="D2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>43140</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>9</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>43172</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>14</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>43173</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="6"/>
+      <c r="C5" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B6" s="3" t="n">
         <v>43152</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="6" t="s">
-        <v>17</v>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="225.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>43172</v>
       </c>
-      <c r="C7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="141.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="225.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>21</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>43235</v>
       </c>
-      <c r="C8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="5"/>
+    </row>
+    <row r="9" customFormat="false" ht="175.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="6"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
+      <c r="C9" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3" t="n">
-        <v>43139</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
@@ -488,13 +462,10 @@
       <c r="B10" s="3" t="n">
         <v>43143</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="6"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -503,28 +474,22 @@
       <c r="B11" s="3" t="n">
         <v>43143</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="148.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="3" t="n">
-        <v>43145</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>6</v>
+        <v>43874</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>30</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -535,13 +500,10 @@
       <c r="B13" s="3" t="n">
         <v>43174</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="0" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>